<commit_message>
Whatever I worked on last night :)
</commit_message>
<xml_diff>
--- a/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
+++ b/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{119CB038-F089-47DD-BCEE-F1E7C45A190A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="2" xr2:uid="{119CB038-F089-47DD-BCEE-F1E7C45A190A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Serial Command Encoding" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,33 +26,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Byte</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+  <si>
+    <t>Packet Type</t>
+  </si>
+  <si>
+    <t>Encoding</t>
+  </si>
+  <si>
+    <t>Millis Timestamp</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Micros Timestamp</t>
+  </si>
+  <si>
+    <t>Data Length</t>
+  </si>
+  <si>
+    <t>Byte 0</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>millis 31:24</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>millis 7:0</t>
+  </si>
+  <si>
+    <t>micros 31:24</t>
+  </si>
+  <si>
+    <t>micros 7:0</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>string[0]</t>
+  </si>
+  <si>
+    <t>string[length-1]</t>
+  </si>
+  <si>
+    <t>Gyro</t>
+  </si>
+  <si>
+    <t>Accel</t>
+  </si>
+  <si>
+    <t>gxh</t>
+  </si>
+  <si>
+    <t>ghl</t>
+  </si>
+  <si>
+    <t>gyh</t>
+  </si>
+  <si>
+    <t>gyl</t>
+  </si>
+  <si>
+    <t>gzh</t>
+  </si>
+  <si>
+    <t>gzl</t>
+  </si>
+  <si>
+    <t>axh</t>
+  </si>
+  <si>
+    <t>axl</t>
+  </si>
+  <si>
+    <t>ayh</t>
+  </si>
+  <si>
+    <t>ayl</t>
+  </si>
+  <si>
+    <t>azh</t>
+  </si>
+  <si>
+    <t>azl</t>
+  </si>
+  <si>
+    <t>Baro_pressure</t>
+  </si>
+  <si>
+    <t>List Files</t>
+  </si>
+  <si>
+    <t>Transmit File</t>
+  </si>
+  <si>
+    <t>Byte 1</t>
+  </si>
+  <si>
+    <t>File Number (uint8)</t>
+  </si>
+  <si>
+    <t>Page 0</t>
+  </si>
+  <si>
+    <t>power_cycles</t>
+  </si>
+  <si>
+    <t>uint32_t</t>
   </si>
   <si>
     <t>Bytes</t>
   </si>
   <si>
-    <t>0-255</t>
-  </si>
-  <si>
-    <t>Reserver</t>
-  </si>
-  <si>
-    <t>Use</t>
-  </si>
-  <si>
-    <t>256-2047</t>
-  </si>
-  <si>
-    <t>File Index</t>
-  </si>
-  <si>
-    <t>File Index Format</t>
-  </si>
-  <si>
-    <t>Bit</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>0:3</t>
+  </si>
+  <si>
+    <t>4:5</t>
+  </si>
+  <si>
+    <t>num_files</t>
+  </si>
+  <si>
+    <t>uint16_t</t>
+  </si>
+  <si>
+    <t>next_file_page</t>
+  </si>
+  <si>
+    <t>num_deletes</t>
+  </si>
+  <si>
+    <t>6:7</t>
+  </si>
+  <si>
+    <t>8:9</t>
   </si>
 </sst>
 </file>
@@ -86,10 +211,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,58 +535,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1597CBE-E4FC-4A6C-A725-026B0CF40E03}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="5" max="12" width="2.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="7.77734375" customWidth="1"/>
     <col min="13" max="20" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1">
         <v>4</v>
+      </c>
+      <c r="I1" s="1">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
       <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -469,15 +714,177 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E5:L5"/>
-    <mergeCell ref="M5:T5"/>
-  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A326D218-A218-4556-A07E-7881EE86149D}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595FFF8B-09A4-4401-BC42-CB05DFAD0607}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added command stuff from the engine controller code base
</commit_message>
<xml_diff>
--- a/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
+++ b/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{119CB038-F089-47DD-BCEE-F1E7C45A190A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{119CB038-F089-47DD-BCEE-F1E7C45A190A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Encoding</t>
   </si>
@@ -103,9 +103,6 @@
     <t>List Files</t>
   </si>
   <si>
-    <t>Transmit File</t>
-  </si>
-  <si>
     <t>Byte 1</t>
   </si>
   <si>
@@ -176,6 +173,21 @@
   </si>
   <si>
     <t>PACKET_TYPE</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Transmit File BIN</t>
+  </si>
+  <si>
+    <t>Transmit File ASCII</t>
+  </si>
+  <si>
+    <t>Wipe disk</t>
+  </si>
+  <si>
+    <t>0xff</t>
   </si>
 </sst>
 </file>
@@ -537,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1597CBE-E4FC-4A6C-A725-026B0CF40E03}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +566,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -595,7 +607,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -621,7 +633,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -647,13 +659,13 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -673,7 +685,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -715,7 +727,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -747,7 +759,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -760,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A326D218-A218-4556-A07E-7881EE86149D}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,34 +784,65 @@
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -823,62 +866,62 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1, 2, 3, 4, 5. 1, 2, 3, 4, 5, 6, 7. This is a bad haiku.
</commit_message>
<xml_diff>
--- a/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
+++ b/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Encoding</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>ax[20:16]</t>
+  </si>
+  <si>
+    <t>END_OF_PAGE</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1597CBE-E4FC-4A6C-A725-026B0CF40E03}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -691,24 +697,26 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -775,6 +783,20 @@
       </c>
       <c r="B7">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>255</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added log functions for some sensors
</commit_message>
<xml_diff>
--- a/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
+++ b/firmware/Flight_Computer_Core/Other Files/Flash Header.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>Encoding</t>
   </si>
@@ -172,15 +172,6 @@
     <t>0xff</t>
   </si>
   <si>
-    <t>ax</t>
-  </si>
-  <si>
-    <t>ay</t>
-  </si>
-  <si>
-    <t>az</t>
-  </si>
-  <si>
     <t>ax[20:16]</t>
   </si>
   <si>
@@ -188,6 +179,45 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>ax[15:8]</t>
+  </si>
+  <si>
+    <t>ax[7:0]</t>
+  </si>
+  <si>
+    <t>ay[20:16]</t>
+  </si>
+  <si>
+    <t>ay[15:8]</t>
+  </si>
+  <si>
+    <t>ay[7:0]</t>
+  </si>
+  <si>
+    <t>az[15:8]</t>
+  </si>
+  <si>
+    <t>az[20:16]</t>
+  </si>
+  <si>
+    <t>az[7:0]</t>
+  </si>
+  <si>
+    <t>data[31:24]</t>
+  </si>
+  <si>
+    <t>data[23:16]</t>
+  </si>
+  <si>
+    <t>data[15:8]</t>
+  </si>
+  <si>
+    <t>data[7:0]</t>
+  </si>
+  <si>
+    <t>nyi</t>
   </si>
 </sst>
 </file>
@@ -550,7 +580,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +591,8 @@
     <col min="6" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="7.77734375" customWidth="1"/>
-    <col min="13" max="20" width="2.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="20" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -610,7 +641,7 @@
         <v>35</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -635,8 +666,8 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -697,7 +728,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
@@ -735,47 +766,41 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -784,10 +809,28 @@
       <c r="B7">
         <v>5</v>
       </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>255</v>

</xml_diff>